<commit_message>
Graficos colunas empilhadas/100% empilhadas
</commit_message>
<xml_diff>
--- a/módulo 07/aula-graficos.xlsx
+++ b/módulo 07/aula-graficos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Mês</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>Insere o novo nome/enter</t>
+  </si>
+  <si>
+    <t>Tabela de dados com legenda</t>
+  </si>
+  <si>
+    <t>Gráfico colunas empilhadas</t>
   </si>
 </sst>
 </file>
@@ -980,8 +986,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="226329936"/>
-        <c:axId val="226330480"/>
+        <c:axId val="565822336"/>
+        <c:axId val="565821248"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1149,7 +1155,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="226329936"/>
+        <c:axId val="565822336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1247,7 +1253,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226330480"/>
+        <c:crossAx val="565821248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1255,7 +1261,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="226330480"/>
+        <c:axId val="565821248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1372,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226329936"/>
+        <c:crossAx val="565822336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1518,7 +1524,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1750,11 +1755,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="414295248"/>
-        <c:axId val="414291984"/>
+        <c:axId val="565812000"/>
+        <c:axId val="565824512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="414295248"/>
+        <c:axId val="565812000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1790,7 +1795,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1857,7 +1861,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414291984"/>
+        <c:crossAx val="565824512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1865,7 +1869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414291984"/>
+        <c:axId val="565824512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +2000,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414295248"/>
+        <c:crossAx val="565812000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2033,7 +2037,6 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2271,11 +2274,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="414295792"/>
-        <c:axId val="414290352"/>
+        <c:axId val="565814176"/>
+        <c:axId val="565823968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="414295792"/>
+        <c:axId val="565814176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2318,7 +2321,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414290352"/>
+        <c:crossAx val="565823968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2326,7 +2329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414290352"/>
+        <c:axId val="565823968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2377,7 +2380,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414295792"/>
+        <c:crossAx val="565814176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2763,6 +2766,1534 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Composição de vendas mensais</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vestuário</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$A$5:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$E$5:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4231.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2955.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3817.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7056.3499999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10828</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6726.24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5004.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7979.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11989.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6407.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6645.54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6696.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alimentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$A$5:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$F$5:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5208.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6192.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4382.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5846.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6063.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6539.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4118.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3117.27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4882.24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10270.380000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12519.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Higiene</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$A$5:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$G$5:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4882.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3237.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4948.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4435.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3031.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4110.4800000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8051.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12097.33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6234.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14951.86</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10874.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8152.4800000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Limpeza</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$A$5:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$H$5:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1953.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1688.8799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>989.66000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2822.5400000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1732.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1307.8800000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1544.34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2637.69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4271.96</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2416.56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1746.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inBase"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="568454816"/>
+        <c:axId val="568449376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="568454816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="568449376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="568449376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0_ ;[Red]\-#,##0\ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="568454816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Gráfico colunas 100% empilhadas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vestuário</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$E$5:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4231.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2955.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3817.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7056.3499999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10828</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6726.24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5004.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7979.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11989.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6407.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6645.54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6696.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alimentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$F$5:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5208.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6192.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4382.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5846.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6063.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6539.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4118.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3117.27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4882.24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10270.380000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12519.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Higiene</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$G$5:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4882.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3237.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4948.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4435.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3031.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4110.4800000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8051.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12097.33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6234.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14951.86</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10874.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8152.4800000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Controle de Vendas'!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Limpeza</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Controle de Vendas'!$H$5:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1953.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1688.8799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>989.66000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2822.5400000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1732.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1307.8800000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1544.34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2637.69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4271.96</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2416.56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1746.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="697379744"/>
+        <c:axId val="697391712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="697379744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697391712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="697391712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697379744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2923,6 +4454,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4622,6 +6233,1016 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -5060,7 +7681,7 @@
         <xdr:cNvPr id="2" name="CaixaDeTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5139,7 +7760,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B530947-99D5-4D97-B33F-F3233C606F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5283,6 +7904,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7301,10 +9982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M17"/>
+  <dimension ref="B1:Y17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q18" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7312,8 +9993,8 @@
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
@@ -7327,8 +10008,11 @@
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Y3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
@@ -7350,8 +10034,11 @@
       <c r="H4" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Y4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
@@ -7379,7 +10066,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -7407,7 +10094,7 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
@@ -7435,7 +10122,7 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
@@ -7463,7 +10150,7 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
@@ -7491,7 +10178,7 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
@@ -7519,7 +10206,7 @@
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
@@ -7547,7 +10234,7 @@
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -7575,7 +10262,7 @@
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
@@ -7603,7 +10290,7 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
@@ -7631,7 +10318,7 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
@@ -7659,7 +10346,7 @@
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>17</v>
       </c>

</xml_diff>